<commit_message>
Scale for Multiple Input Files
</commit_message>
<xml_diff>
--- a/Templates/Log.xlsx
+++ b/Templates/Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://delascasascp-my.sharepoint.com/personal/ro_delascasascp_com/Documents/DLC2P Server/AA Personal/Stefanos/Data Science/Python Projects/CIS Data to Google Earth (Real Time)/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="177" documentId="8_{1893C731-DEF6-9B4A-BCAA-FCE6BE529821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{535062F6-3D85-804C-AAA6-7A34849F31D0}"/>
+  <xr:revisionPtr revIDLastSave="183" documentId="8_{1893C731-DEF6-9B4A-BCAA-FCE6BE529821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC37AEE6-F61F-664E-B00C-ACB8B6185523}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26820" xr2:uid="{FFE7F915-D78A-6246-BD63-347C3DD7C426}"/>
   </bookViews>
@@ -130,7 +130,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -155,6 +155,17 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
@@ -195,7 +206,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -203,9 +214,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -221,9 +229,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -231,6 +236,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -574,188 +600,188 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="25.83203125" customWidth="1"/>
     <col min="2" max="2" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:2" ht="20" customHeight="1">
+      <c r="A1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="12"/>
-    </row>
-    <row r="2" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="B1" s="10"/>
+    </row>
+    <row r="2" spans="1:2" ht="20" customHeight="1">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
-    </row>
-    <row r="3" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="B2" s="5"/>
+    </row>
+    <row r="3" spans="1:2" ht="20" customHeight="1">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6"/>
-    </row>
-    <row r="4" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="B3" s="5"/>
+    </row>
+    <row r="4" spans="1:2" ht="20" customHeight="1">
+      <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6"/>
-    </row>
-    <row r="5" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="B4" s="5"/>
+    </row>
+    <row r="5" spans="1:2" ht="20" customHeight="1">
+      <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7"/>
-    </row>
-    <row r="6" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="B5" s="6"/>
+    </row>
+    <row r="6" spans="1:2" ht="20" customHeight="1">
+      <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8"/>
-    </row>
-    <row r="7" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="B6" s="7"/>
+    </row>
+    <row r="7" spans="1:2" ht="20" customHeight="1">
+      <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2" ht="20" customHeight="1">
+      <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="8"/>
-    </row>
-    <row r="9" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="B8" s="7"/>
+    </row>
+    <row r="9" spans="1:2" ht="20" customHeight="1">
+      <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:2" ht="20" customHeight="1">
+      <c r="A10" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:2" ht="20" customHeight="1">
+      <c r="A11" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="20" customHeight="1">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
+    <row r="13" spans="1:2" ht="20" customHeight="1">
+      <c r="A13" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="12"/>
-    </row>
-    <row r="14" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+      <c r="B13" s="10"/>
+    </row>
+    <row r="14" spans="1:2" ht="20" customHeight="1">
+      <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
+    <row r="15" spans="1:2" ht="20" customHeight="1">
+      <c r="A15" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
+    <row r="16" spans="1:2" ht="20" customHeight="1">
+      <c r="A16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="8"/>
-    </row>
-    <row r="17" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="7"/>
+    </row>
+    <row r="17" spans="1:2" ht="20" customHeight="1">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="s">
+    <row r="18" spans="1:2" ht="20" customHeight="1">
+      <c r="A18" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="12"/>
-    </row>
-    <row r="19" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
+      <c r="B18" s="11"/>
+    </row>
+    <row r="19" spans="1:2" ht="20" customHeight="1">
+      <c r="A19" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="10" t="s">
+      <c r="B19" s="13"/>
+    </row>
+    <row r="20" spans="1:2" ht="20" customHeight="1">
+      <c r="A20" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="4"/>
-    </row>
-    <row r="21" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+      <c r="B20" s="13"/>
+    </row>
+    <row r="21" spans="1:2" ht="20" customHeight="1">
+      <c r="A21" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
+      <c r="B21" s="14"/>
+    </row>
+    <row r="22" spans="1:2" ht="20" customHeight="1">
+      <c r="A22" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
+      <c r="B22" s="14"/>
+    </row>
+    <row r="23" spans="1:2" ht="20" customHeight="1">
+      <c r="A23" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="9"/>
-    </row>
-    <row r="24" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
+      <c r="B23" s="15"/>
+    </row>
+    <row r="24" spans="1:2" ht="20" customHeight="1">
+      <c r="A24" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="5"/>
-    </row>
-    <row r="25" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
+      <c r="B24" s="16"/>
+    </row>
+    <row r="25" spans="1:2" ht="20" customHeight="1">
+      <c r="A25" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="6"/>
-    </row>
-    <row r="26" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="11"/>
-    </row>
-    <row r="27" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="12" t="s">
+      <c r="B25" s="17"/>
+    </row>
+    <row r="26" spans="1:2" ht="20" customHeight="1">
+      <c r="A26" s="9"/>
+    </row>
+    <row r="27" spans="1:2" ht="20" customHeight="1">
+      <c r="A27" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="12"/>
-    </row>
-    <row r="28" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="10" t="s">
+      <c r="B27" s="11"/>
+    </row>
+    <row r="28" spans="1:2" ht="20" customHeight="1">
+      <c r="A28" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="4"/>
-    </row>
-    <row r="29" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
+      <c r="B28" s="13"/>
+    </row>
+    <row r="29" spans="1:2" ht="20" customHeight="1">
+      <c r="A29" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="4"/>
-    </row>
-    <row r="30" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="10" t="s">
+      <c r="B29" s="13"/>
+    </row>
+    <row r="30" spans="1:2" ht="20" customHeight="1">
+      <c r="A30" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B30" s="4"/>
-    </row>
-    <row r="31" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="10" t="s">
+      <c r="B30" s="13"/>
+    </row>
+    <row r="31" spans="1:2" ht="20" customHeight="1">
+      <c r="A31" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="4"/>
+      <c r="B31" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>